<commit_message>
Test suite 600 modified
</commit_message>
<xml_diff>
--- a/test_files/Calculation_hierarchy_members.xlsx
+++ b/test_files/Calculation_hierarchy_members.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="54">
   <si>
     <t>UNARYOPERATOR</t>
   </si>
@@ -19,9 +19,6 @@
     <t>COMPARISONOPERATOR</t>
   </si>
   <si>
-    <t>MEMBERVALUE_3</t>
-  </si>
-  <si>
     <t>CODE</t>
   </si>
   <si>
@@ -46,13 +43,10 @@
     <t>ENDDATE</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>z</t>
+    <t>-</t>
+  </si>
+  <si>
+    <t>&lt;=</t>
   </si>
   <si>
     <t>testcode28</t>
@@ -265,11 +259,11 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="3" width="26.0"/>
-    <col customWidth="1" min="4" max="4" width="18.29"/>
-    <col customWidth="1" min="5" max="5" width="19.0"/>
-    <col customWidth="1" min="6" max="6" width="18.43"/>
-    <col customWidth="1" min="7" max="7" width="18.14"/>
+    <col customWidth="1" min="1" max="2" width="26.0"/>
+    <col customWidth="1" min="3" max="3" width="18.29"/>
+    <col customWidth="1" min="4" max="4" width="19.0"/>
+    <col customWidth="1" min="5" max="5" width="18.43"/>
+    <col customWidth="1" min="6" max="6" width="18.14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -279,7 +273,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -297,392 +291,347 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+      <c r="I2" s="5">
+        <v>42370.0</v>
+      </c>
       <c r="J2" s="5">
-        <v>42370.0</v>
-      </c>
-      <c r="K2" s="5">
         <v>43831.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="I3" s="5">
+        <v>42371.0</v>
+      </c>
       <c r="J3" s="5">
-        <v>42371.0</v>
-      </c>
-      <c r="K3" s="5">
         <v>43832.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+      <c r="I4" s="5">
+        <v>42372.0</v>
+      </c>
       <c r="J4" s="5">
-        <v>42372.0</v>
-      </c>
-      <c r="K4" s="5">
         <v>43833.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="I5" s="5">
+        <v>42373.0</v>
+      </c>
       <c r="J5" s="5">
-        <v>42373.0</v>
-      </c>
-      <c r="K5" s="5">
         <v>43834.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="I6" s="5">
+        <v>42374.0</v>
+      </c>
       <c r="J6" s="5">
-        <v>42374.0</v>
-      </c>
-      <c r="K6" s="5">
         <v>43835.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>31</v>
+      <c r="I7" s="5">
+        <v>42375.0</v>
       </c>
       <c r="J7" s="5">
-        <v>42375.0</v>
-      </c>
-      <c r="K7" s="5">
         <v>43836.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>34</v>
+      <c r="I8" s="5">
+        <v>42376.0</v>
       </c>
       <c r="J8" s="5">
-        <v>42376.0</v>
-      </c>
-      <c r="K8" s="5">
         <v>43837.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>37</v>
+      <c r="I9" s="5">
+        <v>42377.0</v>
       </c>
       <c r="J9" s="5">
-        <v>42377.0</v>
-      </c>
-      <c r="K9" s="5">
         <v>43838.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>40</v>
+      <c r="I10" s="5">
+        <v>42378.0</v>
       </c>
       <c r="J10" s="5">
-        <v>42378.0</v>
-      </c>
-      <c r="K10" s="5">
         <v>43839.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>43</v>
+      <c r="I11" s="5">
+        <v>42379.0</v>
       </c>
       <c r="J11" s="5">
-        <v>42379.0</v>
-      </c>
-      <c r="K11" s="5">
         <v>43840.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>46</v>
+      <c r="I12" s="5">
+        <v>42380.0</v>
       </c>
       <c r="J12" s="5">
-        <v>42380.0</v>
-      </c>
-      <c r="K12" s="5">
         <v>43841.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>49</v>
+      <c r="I13" s="5">
+        <v>42381.0</v>
       </c>
       <c r="J13" s="5">
-        <v>42381.0</v>
-      </c>
-      <c r="K13" s="5">
         <v>43842.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>52</v>
+      <c r="I14" s="5">
+        <v>42382.0</v>
       </c>
       <c r="J14" s="5">
-        <v>42382.0</v>
-      </c>
-      <c r="K14" s="5">
         <v>43843.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>55</v>
+      <c r="I15" s="5">
+        <v>42383.0</v>
       </c>
       <c r="J15" s="5">
-        <v>42383.0</v>
-      </c>
-      <c r="K15" s="5">
         <v>43844.0</v>
       </c>
     </row>

</xml_diff>